<commit_message>
add submitted zip file & add resources/images directory
</commit_message>
<xml_diff>
--- a/hypertext & hypermedia - project 2 - xslt/Informatyka_Józefowicz_Igor_193257_2.xlsx
+++ b/hypertext & hypermedia - project 2 - xslt/Informatyka_Józefowicz_Igor_193257_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20393"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\source\finance-and-investing\hypertext &amp; hypermedia - project 2 - xslt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igorj\source\finance-and-investing\hypertext &amp; hypermedia - project 2 - xslt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3A0281-9E14-4A74-944E-DBF632155023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769C8CF7-F313-430F-AFCC-227AECD0EDD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="25823" windowHeight="13898" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2 projekt" sheetId="4" r:id="rId1"/>
@@ -19,16 +19,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'2 projekt'!$A$2:$D$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1421,18 +1411,18 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.9296875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="79.453125" style="31" customWidth="1"/>
+    <col min="1" max="1" width="79.46484375" style="31" customWidth="1"/>
     <col min="2" max="2" width="6" style="24" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.90625" style="2"/>
-    <col min="6" max="6" width="52.90625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.90625" style="2"/>
+    <col min="3" max="3" width="10.19921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.46484375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.9296875" style="2"/>
+    <col min="6" max="6" width="52.9296875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.9296875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="45" customHeight="1">
@@ -1447,7 +1437,7 @@
       <c r="E1" s="32"/>
       <c r="F1" s="32"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="14.65">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1459,7 +1449,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="30">
+    <row r="3" spans="1:6" ht="29.25">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -1467,14 +1457,14 @@
         <v>1.6</v>
       </c>
       <c r="C3" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="6">
         <f>B3*C3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.65">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1482,14 +1472,14 @@
         <v>0.5</v>
       </c>
       <c r="C4" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" ref="D4:D15" si="0">B4*C4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.65">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -1497,14 +1487,14 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="14.65">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
@@ -1512,14 +1502,14 @@
         <v>0.9</v>
       </c>
       <c r="C6" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14.65">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -1527,14 +1517,14 @@
         <v>0.8</v>
       </c>
       <c r="C7" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="29.25">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -1542,14 +1532,14 @@
         <v>1</v>
       </c>
       <c r="C8" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.9">
       <c r="A9" s="9" t="s">
         <v>30</v>
       </c>
@@ -1557,14 +1547,14 @@
         <v>1</v>
       </c>
       <c r="C9" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="14.65">
       <c r="A10" s="7" t="s">
         <v>21</v>
       </c>
@@ -1572,14 +1562,14 @@
         <v>1</v>
       </c>
       <c r="C10" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="14.65">
       <c r="A11" s="7" t="s">
         <v>22</v>
       </c>
@@ -1587,14 +1577,14 @@
         <v>0.8</v>
       </c>
       <c r="C11" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="14.65">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -1602,14 +1592,14 @@
         <v>0.3</v>
       </c>
       <c r="C12" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="14.65">
       <c r="A13" s="7" t="s">
         <v>35</v>
       </c>
@@ -1617,14 +1607,14 @@
         <v>0.6</v>
       </c>
       <c r="C13" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="14.65">
       <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
@@ -1632,14 +1622,14 @@
         <v>0.8</v>
       </c>
       <c r="C14" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="14.65">
       <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
@@ -1647,14 +1637,14 @@
         <v>0.8</v>
       </c>
       <c r="C15" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="14.65">
       <c r="A16" s="10" t="s">
         <v>25</v>
       </c>
@@ -1665,16 +1655,16 @@
       <c r="C16" s="26"/>
       <c r="D16" s="11">
         <f>SUM(D3:D15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>10.600000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.65">
       <c r="A17" s="4"/>
       <c r="B17" s="8"/>
       <c r="C17" s="25"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" ht="14.65">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1682,7 +1672,7 @@
       <c r="C18" s="25"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" ht="30">
+    <row r="19" spans="1:4" ht="14.65">
       <c r="A19" s="7" t="s">
         <v>14</v>
       </c>
@@ -1697,7 +1687,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30">
+    <row r="20" spans="1:4" ht="29.25">
       <c r="A20" s="7" t="s">
         <v>15</v>
       </c>
@@ -1712,7 +1702,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30">
+    <row r="21" spans="1:4" ht="29.25">
       <c r="A21" s="7" t="s">
         <v>31</v>
       </c>
@@ -1727,7 +1717,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30">
+    <row r="22" spans="1:4" ht="29.25">
       <c r="A22" s="7" t="s">
         <v>36</v>
       </c>
@@ -1742,7 +1732,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30">
+    <row r="23" spans="1:4" ht="29.25">
       <c r="A23" s="7" t="s">
         <v>37</v>
       </c>
@@ -1757,7 +1747,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15">
+    <row r="24" spans="1:4" ht="14.65">
       <c r="A24" s="12" t="s">
         <v>16</v>
       </c>
@@ -1772,7 +1762,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15">
+    <row r="25" spans="1:4" ht="14.65">
       <c r="A25" s="12" t="s">
         <v>17</v>
       </c>
@@ -1787,7 +1777,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15">
+    <row r="26" spans="1:4" ht="14.65">
       <c r="A26" s="12" t="s">
         <v>18</v>
       </c>
@@ -1802,7 +1792,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15">
+    <row r="27" spans="1:4" ht="14.65">
       <c r="A27" s="12" t="s">
         <v>19</v>
       </c>
@@ -1817,7 +1807,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" ht="14.65">
       <c r="A28" s="10" t="s">
         <v>26</v>
       </c>
@@ -1842,7 +1832,7 @@
       <c r="C29" s="27"/>
       <c r="D29" s="13">
         <f>D28+D16</f>
-        <v>4.3999999999999995</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1855,7 +1845,7 @@
       <c r="A31" s="22"/>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:4" ht="15.5">
+    <row r="32" spans="1:4" ht="15.4">
       <c r="A32" s="17" t="s">
         <v>27</v>
       </c>
@@ -1868,7 +1858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.5">
+    <row r="33" spans="1:4" ht="15.4">
       <c r="A33" s="17" t="s">
         <v>28</v>
       </c>
@@ -1881,7 +1871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.5">
+    <row r="34" spans="1:4" ht="15.4">
       <c r="A34" s="17" t="s">
         <v>29</v>
       </c>
@@ -1894,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.5">
+    <row r="35" spans="1:4" ht="15.4">
       <c r="A35" s="17" t="s">
         <v>32</v>
       </c>
@@ -1925,7 +1915,7 @@
       <c r="C37" s="30"/>
       <c r="D37" s="21">
         <f>D29+D32+D33+D34+D35+D30</f>
-        <v>4.3999999999999995</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:4">

</xml_diff>